<commit_message>
Updated tool with basic ROI calculation added
</commit_message>
<xml_diff>
--- a/Tools/CampaignEvaluationTool.xlsx
+++ b/Tools/CampaignEvaluationTool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/53bc5ca0560a0124/DataSci/AB_Testing/Tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{C40AAB96-183B-46BB-AF9B-12671DB2F738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62A3BAEE-02B9-4BFF-9926-314CE0AC7C9D}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{C40AAB96-183B-46BB-AF9B-12671DB2F738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA3F6AA1-EA5E-4220-9373-35CF4EF02F41}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="1790" windowWidth="21600" windowHeight="11300" xr2:uid="{A67C6000-0767-4B4F-BF88-236B4B6B48DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A67C6000-0767-4B4F-BF88-236B4B6B48DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Control Group Conversion</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t>Input Values - adjust for planned campaigns</t>
+  </si>
+  <si>
+    <t>Costs</t>
+  </si>
+  <si>
+    <t>Extra Revenue</t>
+  </si>
+  <si>
+    <t>ROI</t>
   </si>
 </sst>
 </file>
@@ -108,7 +117,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -210,7 +219,7 @@
     <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -231,7 +240,7 @@
     <xf numFmtId="2" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="3" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -580,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C073A1-5A73-4475-A531-FADDAB15F86A}">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +606,7 @@
     <col min="15" max="15" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -652,8 +661,17 @@
       <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
@@ -721,7 +739,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>8.9999999999999993E-3</v>
       </c>
@@ -790,7 +808,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>8.9999999999999993E-3</v>
       </c>
@@ -859,23 +877,191 @@
         <v>Yes</v>
       </c>
       <c r="S4">
-        <f>P4*C4*24*15</f>
-        <v>24299.999999999993</v>
+        <f>P4*0.8</f>
+        <v>18000</v>
+      </c>
+      <c r="T4">
+        <f>10*24*P4*C4</f>
+        <v>16199.999999999996</v>
+      </c>
+      <c r="U4">
+        <f>T4/S4</f>
+        <v>0.8999999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="B5" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C5" s="8">
+        <f>A5-B5</f>
+        <v>3.9999999999999992E-3</v>
+      </c>
+      <c r="D5" s="9">
+        <f t="shared" ref="D5" si="1">A5/B5-1</f>
+        <v>0.79999999999999982</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="G5" s="11">
+        <f>(A5*P5+B5*Q5)/O5</f>
+        <v>7.9999999999999984E-3</v>
+      </c>
+      <c r="H5" s="11">
+        <f>_xlfn.NORM.S.INV(1-E5)</f>
+        <v>1.6448536269514715</v>
+      </c>
+      <c r="I5" s="11">
+        <f>_xlfn.NORM.S.INV(F5)</f>
+        <v>0.84162123357291474</v>
+      </c>
+      <c r="J5" s="11">
+        <f>SQRT(G5*(1-G5)*(1/Q5+1/P5))</f>
+        <v>1.1877897307370712E-3</v>
+      </c>
+      <c r="K5" s="12">
+        <f>(A5-B5)/J5</f>
+        <v>3.3675994130020293</v>
+      </c>
+      <c r="L5" s="12">
+        <f>H5+I5</f>
+        <v>2.4864748605243863</v>
+      </c>
+      <c r="M5" s="13">
+        <f>(_xlfn.NORM.S.DIST(K5,TRUE))</f>
+        <v>0.99962087158359914</v>
+      </c>
+      <c r="N5" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="O5" s="5">
+        <v>30000</v>
+      </c>
+      <c r="P5" s="14">
+        <f>O5*N5</f>
+        <v>22500</v>
+      </c>
+      <c r="Q5" s="14">
+        <f>O5-P5</f>
+        <v>7500</v>
+      </c>
+      <c r="R5" s="15" t="str">
+        <f>IF(K5&gt;L5,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+      <c r="S5">
+        <f>P5*0.8</f>
+        <v>18000</v>
+      </c>
+      <c r="T5">
+        <f t="shared" ref="T5:T6" si="2">10*24*P5*C5</f>
+        <v>21599.999999999996</v>
+      </c>
+      <c r="U5">
+        <f>T5/S5</f>
+        <v>1.1999999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>1.2E-2</v>
+      </c>
+      <c r="B6" s="6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C6" s="8">
+        <f>A6-B6</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" ref="D6" si="3">A6/B6-1</f>
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="G6" s="11">
+        <f>(A6*P6+B6*Q6)/O6</f>
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="H6" s="11">
+        <f>_xlfn.NORM.S.INV(1-E6)</f>
+        <v>1.6448536269514715</v>
+      </c>
+      <c r="I6" s="11">
+        <f>_xlfn.NORM.S.INV(F6)</f>
+        <v>0.84162123357291474</v>
+      </c>
+      <c r="J6" s="11">
+        <f>SQRT(G6*(1-G6)*(1/Q6+1/P6))</f>
+        <v>1.1660725760111385E-3</v>
+      </c>
+      <c r="K6" s="12">
+        <f>(A6-B6)/J6</f>
+        <v>3.4303182171413931</v>
+      </c>
+      <c r="L6" s="12">
+        <f>H6+I6</f>
+        <v>2.4864748605243863</v>
+      </c>
+      <c r="M6" s="13">
+        <f>(_xlfn.NORM.S.DIST(K6,TRUE))</f>
+        <v>0.99969856311285876</v>
+      </c>
+      <c r="N6" s="7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="O6" s="5">
+        <v>30000</v>
+      </c>
+      <c r="P6" s="14">
+        <f>O6*N6</f>
+        <v>16500</v>
+      </c>
+      <c r="Q6" s="14">
+        <f>O6-P6</f>
+        <v>13500</v>
+      </c>
+      <c r="R6" s="15" t="str">
+        <f>IF(K6&gt;L6,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+      <c r="S6">
+        <f>P6*0.8</f>
+        <v>13200</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="2"/>
+        <v>15840</v>
+      </c>
+      <c r="U6">
+        <f>T6/S6</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Update to walkthrough notebook - story now polished
</commit_message>
<xml_diff>
--- a/Tools/CampaignEvaluationTool.xlsx
+++ b/Tools/CampaignEvaluationTool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/53bc5ca0560a0124/DataSci/AB_Testing/Tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{C40AAB96-183B-46BB-AF9B-12671DB2F738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA3F6AA1-EA5E-4220-9373-35CF4EF02F41}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{C40AAB96-183B-46BB-AF9B-12671DB2F738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A435E429-E727-4439-878D-46CEFE46232C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A67C6000-0767-4B4F-BF88-236B4B6B48DD}"/>
   </bookViews>
@@ -589,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C073A1-5A73-4475-A531-FADDAB15F86A}">
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +961,7 @@
         <v>18000</v>
       </c>
       <c r="T5">
-        <f t="shared" ref="T5:T6" si="2">10*24*P5*C5</f>
+        <f t="shared" ref="T5:T7" si="2">10*24*P5*C5</f>
         <v>21599.999999999996</v>
       </c>
       <c r="U5">
@@ -971,18 +971,18 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <v>1.2E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="B6" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C6" s="8">
         <f>A6-B6</f>
-        <v>4.0000000000000001E-3</v>
+        <v>4.9999999999999992E-3</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" ref="D6" si="3">A6/B6-1</f>
-        <v>0.5</v>
+        <v>0.625</v>
       </c>
       <c r="E6" s="10">
         <v>0.05</v>
@@ -992,7 +992,7 @@
       </c>
       <c r="G6" s="11">
         <f>(A6*P6+B6*Q6)/O6</f>
-        <v>1.0200000000000001E-2</v>
+        <v>1.0749999999999999E-2</v>
       </c>
       <c r="H6" s="11">
         <f>_xlfn.NORM.S.INV(1-E6)</f>
@@ -1004,11 +1004,11 @@
       </c>
       <c r="J6" s="11">
         <f>SQRT(G6*(1-G6)*(1/Q6+1/P6))</f>
-        <v>1.1660725760111385E-3</v>
+        <v>1.1967654217713154E-3</v>
       </c>
       <c r="K6" s="12">
         <f>(A6-B6)/J6</f>
-        <v>3.4303182171413931</v>
+        <v>4.1779281963206882</v>
       </c>
       <c r="L6" s="12">
         <f>H6+I6</f>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="M6" s="13">
         <f>(_xlfn.NORM.S.DIST(K6,TRUE))</f>
-        <v>0.99969856311285876</v>
+        <v>0.99998529117562895</v>
       </c>
       <c r="N6" s="7">
         <v>0.55000000000000004</v>
@@ -1037,33 +1037,173 @@
         <v>Yes</v>
       </c>
       <c r="S6">
-        <f>P6*0.8</f>
-        <v>13200</v>
+        <f>P6*1</f>
+        <v>16500</v>
       </c>
       <c r="T6">
         <f t="shared" si="2"/>
-        <v>15840</v>
+        <v>19799.999999999996</v>
       </c>
       <c r="U6">
         <f>T6/S6</f>
-        <v>1.2</v>
+        <v>1.1999999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" t="s">
-        <v>20</v>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>1.2E-2</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C7" s="8">
+        <f>A7-B7</f>
+        <v>2E-3</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" ref="D7" si="4">A7/B7-1</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="G7" s="11">
+        <f>(A7*P7+B7*Q7)/O7</f>
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="H7" s="11">
+        <f>_xlfn.NORM.S.INV(1-E7)</f>
+        <v>1.6448536269514715</v>
+      </c>
+      <c r="I7" s="11">
+        <f>_xlfn.NORM.S.INV(F7)</f>
+        <v>0.84162123357291474</v>
+      </c>
+      <c r="J7" s="11">
+        <f>SQRT(G7*(1-G7)*(1/Q7+1/P7))</f>
+        <v>1.0117806086301516E-3</v>
+      </c>
+      <c r="K7" s="12">
+        <f>(A7-B7)/J7</f>
+        <v>1.9767131164015856</v>
+      </c>
+      <c r="L7" s="12">
+        <f>H7+I7</f>
+        <v>2.4864748605243863</v>
+      </c>
+      <c r="M7" s="13">
+        <f>(_xlfn.NORM.S.DIST(K7,TRUE))</f>
+        <v>0.9759629663286935</v>
+      </c>
+      <c r="N7" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="O7" s="5">
+        <v>70000</v>
+      </c>
+      <c r="P7" s="14">
+        <f>O7*N7</f>
+        <v>56000</v>
+      </c>
+      <c r="Q7" s="14">
+        <f>O7-P7</f>
+        <v>14000</v>
+      </c>
+      <c r="R7" s="15" t="str">
+        <f>IF(K7&gt;L7,"Yes","No")</f>
+        <v>No</v>
+      </c>
+      <c r="T7">
+        <f>10*24*P7*C7</f>
+        <v>26880</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>1.2E-2</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C8" s="8">
+        <f>A8-B8</f>
+        <v>2E-3</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" ref="D8" si="5">A8/B8-1</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="G8" s="11">
+        <f>(A8*P8+B8*Q8)/O8</f>
+        <v>1.18E-2</v>
+      </c>
+      <c r="H8" s="11">
+        <f>_xlfn.NORM.S.INV(1-E8)</f>
+        <v>1.6448536269514715</v>
+      </c>
+      <c r="I8" s="11">
+        <f>_xlfn.NORM.S.INV(F8)</f>
+        <v>0.84162123357291474</v>
+      </c>
+      <c r="J8" s="11">
+        <f>SQRT(G8*(1-G8)*(1/Q8+1/P8))</f>
+        <v>1.3604831074711238E-3</v>
+      </c>
+      <c r="K8" s="12">
+        <f>(A8-B8)/J8</f>
+        <v>1.4700660294986059</v>
+      </c>
+      <c r="L8" s="12">
+        <f>H8+I8</f>
+        <v>2.4864748605243863</v>
+      </c>
+      <c r="M8" s="13">
+        <f>(_xlfn.NORM.S.DIST(K8,TRUE))</f>
+        <v>0.92922806416107973</v>
+      </c>
+      <c r="N8" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="O8" s="5">
+        <v>70000</v>
+      </c>
+      <c r="P8" s="14">
+        <f>O8*N8</f>
+        <v>63000</v>
+      </c>
+      <c r="Q8" s="14">
+        <f>O8-P8</f>
+        <v>7000</v>
+      </c>
+      <c r="R8" s="15" t="str">
+        <f>IF(K8&gt;L8,"Yes","No")</f>
+        <v>No</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="4"/>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="3"/>
       <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>